<commit_message>
Update BAC-23-Ficha técnica de una acción estratégica.xlsx
</commit_message>
<xml_diff>
--- a/HT-6/BAC-23-Ficha técnica de una acción estratégica.xlsx
+++ b/HT-6/BAC-23-Ficha técnica de una acción estratégica.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juan/Documents/Universidad/2022-20/arquiemp/repo/arquiemp/HT-6/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B455EB5-D753-1642-9586-2893F61346D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F65068C-E188-3E46-93BD-4FD95982125D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{6D2ADF59-F33A-44E3-88FB-8431094B32CC}"/>
+    <workbookView xWindow="31360" yWindow="-3740" windowWidth="28800" windowHeight="17500" firstSheet="1" activeTab="13" xr2:uid="{6D2ADF59-F33A-44E3-88FB-8431094B32CC}"/>
   </bookViews>
   <sheets>
     <sheet name="BAC-23-1" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,15 @@
     <sheet name="BAC-23-3" sheetId="7" r:id="rId3"/>
     <sheet name="BAC-23-4" sheetId="8" r:id="rId4"/>
     <sheet name="BAC-23-5" sheetId="9" r:id="rId5"/>
+    <sheet name="BAC-23-6" sheetId="11" r:id="rId6"/>
+    <sheet name="BAC-23-7" sheetId="12" r:id="rId7"/>
+    <sheet name="BAC-23-8" sheetId="13" r:id="rId8"/>
+    <sheet name="BAC-23-9" sheetId="14" r:id="rId9"/>
+    <sheet name="BAC-23-10" sheetId="15" r:id="rId10"/>
+    <sheet name="BAC-23-11" sheetId="16" r:id="rId11"/>
+    <sheet name="BAC-23-12" sheetId="17" r:id="rId12"/>
+    <sheet name="BAC-23-13" sheetId="18" r:id="rId13"/>
+    <sheet name="BAC-23-14" sheetId="19" r:id="rId14"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="14">
   <si>
     <t>ID</t>
   </si>
@@ -515,8 +524,838 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4ABDEE2F-9DA5-4F4F-A9BF-B9BEA22ACD0E}">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="170" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="170" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="7.83203125" customWidth="1"/>
+    <col min="2" max="2" width="26.6640625" customWidth="1"/>
+    <col min="3" max="6" width="15" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="1"/>
+    </row>
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.15">
+      <c r="A5" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A6" s="7"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A7" s="2"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A8" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+    </row>
+    <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A9" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A10" s="7"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A11" s="7"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A12" s="7"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A13" s="7"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A14" s="7"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A15" s="7"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A16" s="7"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A17" s="7"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A8:F8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC6F8770-7D2A-FE43-B9B1-7515A53F4969}">
+  <dimension ref="A1:F17"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="7.83203125" customWidth="1"/>
+    <col min="2" max="2" width="26.6640625" customWidth="1"/>
+    <col min="3" max="6" width="15" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="1"/>
+    </row>
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.15">
+      <c r="A5" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A6" s="7"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A7" s="2"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A8" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+    </row>
+    <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A9" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A10" s="7"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A11" s="7"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A12" s="7"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A13" s="7"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A14" s="7"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A15" s="7"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A16" s="7"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A17" s="7"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A8:F8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF4E0936-63B9-234E-BBE9-144C07C71A14}">
+  <dimension ref="A1:F17"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="7.83203125" customWidth="1"/>
+    <col min="2" max="2" width="26.6640625" customWidth="1"/>
+    <col min="3" max="6" width="15" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="1"/>
+    </row>
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.15">
+      <c r="A5" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A6" s="7"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A7" s="2"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A8" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+    </row>
+    <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A9" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A10" s="7"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A11" s="7"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A12" s="7"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A13" s="7"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A14" s="7"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A15" s="7"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A16" s="7"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A17" s="7"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A8:F8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA5D5DA9-6D7A-B042-A069-61E3E8131A55}">
+  <dimension ref="A1:F17"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="P40" sqref="P40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="7.83203125" customWidth="1"/>
+    <col min="2" max="2" width="26.6640625" customWidth="1"/>
+    <col min="3" max="6" width="15" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="1"/>
+    </row>
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.15">
+      <c r="A5" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A6" s="7"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A7" s="2"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A8" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+    </row>
+    <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A9" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A10" s="7"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A11" s="7"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A12" s="7"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A13" s="7"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A14" s="7"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A15" s="7"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A16" s="7"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A17" s="7"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A8:F8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B22E0380-33E0-F14F-B782-F6367023B4CC}">
+  <dimension ref="A1:F17"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="P39" sqref="P39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="7.83203125" customWidth="1"/>
+    <col min="2" max="2" width="26.6640625" customWidth="1"/>
+    <col min="3" max="6" width="15" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="1"/>
+    </row>
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.15">
+      <c r="A5" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A6" s="7"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A7" s="2"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A8" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+    </row>
+    <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A9" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A10" s="7"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A11" s="7"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A12" s="7"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A13" s="7"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A14" s="7"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A15" s="7"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A16" s="7"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A17" s="7"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A8:F8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46C5CF9B-D9BE-5542-B3EA-979302F26D14}">
+  <dimension ref="A1:F17"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -1339,4 +2178,668 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00EDEF22-2DAF-F74D-BBF5-044C4F22FF21}">
+  <dimension ref="A1:F17"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="7.83203125" customWidth="1"/>
+    <col min="2" max="2" width="26.6640625" customWidth="1"/>
+    <col min="3" max="6" width="15" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="1"/>
+    </row>
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.15">
+      <c r="A5" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A6" s="7"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A7" s="2"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A8" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+    </row>
+    <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A9" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A10" s="7"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A11" s="7"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A12" s="7"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A13" s="7"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A14" s="7"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A15" s="7"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A16" s="7"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A17" s="7"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A8:F8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62DC724D-1174-B04F-9A49-0FEE030861B3}">
+  <dimension ref="A1:F17"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="7.83203125" customWidth="1"/>
+    <col min="2" max="2" width="26.6640625" customWidth="1"/>
+    <col min="3" max="6" width="15" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="1"/>
+    </row>
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.15">
+      <c r="A5" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A6" s="7"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A7" s="2"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A8" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+    </row>
+    <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A9" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A10" s="7"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A11" s="7"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A12" s="7"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A13" s="7"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A14" s="7"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A15" s="7"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A16" s="7"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A17" s="7"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A8:F8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4ED998C-70E0-5643-81EC-F018CCEF7BD7}">
+  <dimension ref="A1:F17"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="7.83203125" customWidth="1"/>
+    <col min="2" max="2" width="26.6640625" customWidth="1"/>
+    <col min="3" max="6" width="15" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="1"/>
+    </row>
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.15">
+      <c r="A5" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A6" s="7"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A7" s="2"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A8" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+    </row>
+    <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A9" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A10" s="7"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A11" s="7"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A12" s="7"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A13" s="7"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A14" s="7"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A15" s="7"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A16" s="7"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A17" s="7"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A8:F8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CF326E3-3636-F74B-AF46-2CCBBAFD2D5A}">
+  <dimension ref="A1:F17"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="7.83203125" customWidth="1"/>
+    <col min="2" max="2" width="26.6640625" customWidth="1"/>
+    <col min="3" max="6" width="15" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="1"/>
+    </row>
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.15">
+      <c r="A5" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A6" s="7"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A7" s="2"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A8" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+    </row>
+    <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A9" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A10" s="7"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A11" s="7"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A12" s="7"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A13" s="7"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A14" s="7"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A15" s="7"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A16" s="7"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A17" s="7"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A8:F8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>